<commit_message>
13-Apr-2024: App and xlsx files were modified to support test_batch_no.
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41ED70E-F304-1A4F-ACCB-5E312308EF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82757323-FE83-D34C-A0DA-71749682C315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
+    <workbookView xWindow="11740" yWindow="9400" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>cand_no</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Steve</t>
+  </si>
+  <si>
+    <t>batch_no</t>
   </si>
 </sst>
 </file>
@@ -453,82 +456,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC3D66E-995A-6B4C-88A0-411F10AD1979}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3333</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>98765432</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3333</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>65432109</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3333</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>90156789</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3333</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>24484568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3334</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>98765432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3334</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>65432109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
14-Apr-2024: Administrator functions were implemented.
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82757323-FE83-D34C-A0DA-71749682C315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8489EB76-29F1-0E4E-9A5D-E1F01ED5B965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="9400" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
+    <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>cand_no</t>
   </si>
@@ -456,9 +456,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC3D66E-995A-6B4C-88A0-411F10AD1979}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -581,6 +583,74 @@
         <v>65432109</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6666</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>90156789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6666</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>24484568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5555</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>98765432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5555</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>65432109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
15-Apr-2024: Example question bank file was added.
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8489EB76-29F1-0E4E-9A5D-E1F01ED5B965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C548564E-45EF-7545-B241-F61ED44C8904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,7 +483,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>3333</v>
+        <v>1111</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3333</v>
+        <v>1111</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3333</v>
+        <v>1111</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3333</v>
+        <v>1112</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3334</v>
+        <v>1112</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3334</v>
+        <v>1113</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6666</v>
+        <v>1113</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>6666</v>
+        <v>1113</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>5555</v>
+        <v>1114</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5555</v>
+        <v>1114</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
19-Apr-2024: Rewrite the app to support multiplex trades.
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C548564E-45EF-7545-B241-F61ED44C8904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57EC8B5-816E-1647-93EE-91C94CBABBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{33DC2F0A-A837-CC48-AC78-A8FB66671071}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>cand_no</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>batch_no</t>
+  </si>
+  <si>
+    <t>trade</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>VM</t>
+  </si>
+  <si>
+    <t>VM98765</t>
+  </si>
+  <si>
+    <t>VM54321</t>
+  </si>
+  <si>
+    <t>VM666666</t>
+  </si>
+  <si>
+    <t>VM12345</t>
   </si>
 </sst>
 </file>
@@ -456,198 +477,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC3D66E-995A-6B4C-88A0-411F10AD1979}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
         <v>1111</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>98765432</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
         <v>1111</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>65432109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
         <v>1111</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>90156789</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
         <v>1112</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>24484568</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
         <v>1112</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>98765432</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
         <v>1113</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>65432109</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
         <v>1113</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>90156789</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
         <v>1113</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>24484568</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
         <v>1114</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
       <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>98765432</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
         <v>1114</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
       <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>65432109</v>
       </c>
     </row>

</xml_diff>